<commit_message>
Make the values consistent
</commit_message>
<xml_diff>
--- a/web/static/documents/fichier_exemple_complet_ma_cantine.xlsx
+++ b/web/static/documents/fichier_exemple_complet_ma_cantine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenfrancesroot/Develop/ma-cantine/web/static/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3976D2C4-F630-E14F-AC88-7DDC7C6FD46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A719069F-6440-274C-A809-0A582332CD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="39780" windowHeight="21180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -260,7 +260,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -308,45 +308,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -383,6 +361,40 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,7 +780,7 @@
   <dimension ref="A1:DW11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CO1" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CJ1" sqref="CJ1:CQ1"/>
+      <selection activeCell="CW24" sqref="CW24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -795,7 +807,7 @@
     <col min="20" max="20" width="38.6640625" customWidth="1"/>
     <col min="21" max="21" width="31" customWidth="1"/>
     <col min="22" max="22" width="10" customWidth="1"/>
-    <col min="23" max="23" width="43.33203125" style="12" customWidth="1"/>
+    <col min="23" max="23" width="43.33203125" style="1" customWidth="1"/>
     <col min="24" max="24" width="39.33203125" customWidth="1"/>
     <col min="25" max="25" width="35.5" customWidth="1"/>
     <col min="26" max="26" width="32.83203125" customWidth="1"/>
@@ -803,7 +815,7 @@
     <col min="28" max="28" width="38.6640625" customWidth="1"/>
     <col min="29" max="29" width="31" customWidth="1"/>
     <col min="30" max="30" width="10" customWidth="1"/>
-    <col min="31" max="31" width="43.33203125" style="12" customWidth="1"/>
+    <col min="31" max="31" width="43.33203125" style="1" customWidth="1"/>
     <col min="32" max="32" width="39.33203125" customWidth="1"/>
     <col min="33" max="33" width="35.5" customWidth="1"/>
     <col min="34" max="34" width="32.83203125" customWidth="1"/>
@@ -811,7 +823,7 @@
     <col min="36" max="36" width="38.6640625" customWidth="1"/>
     <col min="37" max="37" width="31" customWidth="1"/>
     <col min="38" max="38" width="10" customWidth="1"/>
-    <col min="39" max="39" width="43.33203125" style="12" customWidth="1"/>
+    <col min="39" max="39" width="43.33203125" style="1" customWidth="1"/>
     <col min="40" max="40" width="39.33203125" customWidth="1"/>
     <col min="41" max="41" width="35.5" customWidth="1"/>
     <col min="42" max="42" width="32.83203125" customWidth="1"/>
@@ -819,7 +831,7 @@
     <col min="44" max="44" width="38.6640625" customWidth="1"/>
     <col min="45" max="45" width="31" customWidth="1"/>
     <col min="46" max="46" width="10" customWidth="1"/>
-    <col min="47" max="47" width="43.33203125" style="12" customWidth="1"/>
+    <col min="47" max="47" width="43.33203125" style="1" customWidth="1"/>
     <col min="48" max="48" width="39.33203125" customWidth="1"/>
     <col min="49" max="49" width="35.5" customWidth="1"/>
     <col min="50" max="50" width="32.83203125" customWidth="1"/>
@@ -827,7 +839,7 @@
     <col min="52" max="52" width="38.6640625" customWidth="1"/>
     <col min="53" max="53" width="31" customWidth="1"/>
     <col min="54" max="54" width="10" customWidth="1"/>
-    <col min="55" max="55" width="43.33203125" style="12" customWidth="1"/>
+    <col min="55" max="55" width="43.33203125" style="1" customWidth="1"/>
     <col min="56" max="56" width="39.33203125" customWidth="1"/>
     <col min="57" max="57" width="35.5" customWidth="1"/>
     <col min="58" max="58" width="32.83203125" customWidth="1"/>
@@ -835,7 +847,7 @@
     <col min="60" max="60" width="38.6640625" customWidth="1"/>
     <col min="61" max="61" width="31" customWidth="1"/>
     <col min="62" max="62" width="10" customWidth="1"/>
-    <col min="63" max="63" width="43.33203125" style="12" customWidth="1"/>
+    <col min="63" max="63" width="43.33203125" style="1" customWidth="1"/>
     <col min="64" max="64" width="39.33203125" customWidth="1"/>
     <col min="65" max="65" width="35.5" customWidth="1"/>
     <col min="66" max="66" width="32.83203125" customWidth="1"/>
@@ -843,7 +855,7 @@
     <col min="68" max="68" width="38.6640625" customWidth="1"/>
     <col min="69" max="69" width="31" customWidth="1"/>
     <col min="70" max="70" width="10" customWidth="1"/>
-    <col min="71" max="71" width="43.33203125" style="12" customWidth="1"/>
+    <col min="71" max="71" width="43.33203125" style="1" customWidth="1"/>
     <col min="72" max="72" width="39.33203125" customWidth="1"/>
     <col min="73" max="73" width="35.5" customWidth="1"/>
     <col min="74" max="74" width="32.83203125" customWidth="1"/>
@@ -851,7 +863,7 @@
     <col min="76" max="76" width="38.6640625" customWidth="1"/>
     <col min="77" max="77" width="31" customWidth="1"/>
     <col min="78" max="78" width="10" customWidth="1"/>
-    <col min="79" max="79" width="43.33203125" style="12" customWidth="1"/>
+    <col min="79" max="79" width="43.33203125" style="1" customWidth="1"/>
     <col min="80" max="80" width="39.33203125" customWidth="1"/>
     <col min="81" max="81" width="35.5" customWidth="1"/>
     <col min="82" max="82" width="32.83203125" customWidth="1"/>
@@ -859,7 +871,7 @@
     <col min="84" max="84" width="38.6640625" customWidth="1"/>
     <col min="85" max="85" width="31" customWidth="1"/>
     <col min="86" max="86" width="10" customWidth="1"/>
-    <col min="87" max="87" width="43.33203125" style="12" customWidth="1"/>
+    <col min="87" max="87" width="43.33203125" style="1" customWidth="1"/>
     <col min="88" max="88" width="39.33203125" customWidth="1"/>
     <col min="89" max="89" width="35.5" customWidth="1"/>
     <col min="90" max="90" width="32.83203125" customWidth="1"/>
@@ -867,8 +879,9 @@
     <col min="92" max="92" width="38.6640625" customWidth="1"/>
     <col min="93" max="93" width="31" customWidth="1"/>
     <col min="94" max="94" width="10" customWidth="1"/>
-    <col min="95" max="95" width="43.33203125" style="12" customWidth="1"/>
-    <col min="96" max="103" width="43.33203125" style="37" customWidth="1"/>
+    <col min="95" max="95" width="43.33203125" style="1" customWidth="1"/>
+    <col min="96" max="102" width="43.33203125" style="26" customWidth="1"/>
+    <col min="103" max="103" width="43.33203125" style="1" customWidth="1"/>
     <col min="104" max="104" width="39.33203125" customWidth="1"/>
     <col min="105" max="105" width="35.5" customWidth="1"/>
     <col min="106" max="106" width="32.83203125" customWidth="1"/>
@@ -876,7 +889,7 @@
     <col min="108" max="108" width="38.6640625" customWidth="1"/>
     <col min="109" max="109" width="31" customWidth="1"/>
     <col min="110" max="110" width="10" customWidth="1"/>
-    <col min="111" max="111" width="43.33203125" style="12" customWidth="1"/>
+    <col min="111" max="111" width="43.33203125" style="1" customWidth="1"/>
     <col min="112" max="112" width="39.33203125" customWidth="1"/>
     <col min="113" max="113" width="35.5" customWidth="1"/>
     <col min="114" max="114" width="32.83203125" customWidth="1"/>
@@ -884,7 +897,7 @@
     <col min="116" max="116" width="38.6640625" customWidth="1"/>
     <col min="117" max="117" width="31" customWidth="1"/>
     <col min="118" max="118" width="10" customWidth="1"/>
-    <col min="119" max="119" width="43.33203125" style="12" customWidth="1"/>
+    <col min="119" max="119" width="43.33203125" style="1" customWidth="1"/>
     <col min="120" max="120" width="39.33203125" customWidth="1"/>
     <col min="121" max="121" width="35.5" customWidth="1"/>
     <col min="122" max="122" width="32.83203125" customWidth="1"/>
@@ -895,531 +908,531 @@
     <col min="127" max="127" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:127" s="13" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O1" s="14" t="s">
+    <row r="1" spans="1:127" s="2" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="10" t="s">
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="9" t="s">
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="9"/>
-      <c r="AL1" s="9"/>
-      <c r="AM1" s="9"/>
-      <c r="AN1" s="8" t="s">
+      <c r="AG1" s="41"/>
+      <c r="AH1" s="41"/>
+      <c r="AI1" s="41"/>
+      <c r="AJ1" s="41"/>
+      <c r="AK1" s="41"/>
+      <c r="AL1" s="41"/>
+      <c r="AM1" s="41"/>
+      <c r="AN1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="AO1" s="8"/>
-      <c r="AP1" s="8"/>
-      <c r="AQ1" s="8"/>
-      <c r="AR1" s="8"/>
-      <c r="AS1" s="8"/>
-      <c r="AT1" s="8"/>
-      <c r="AU1" s="8"/>
-      <c r="AV1" s="7" t="s">
+      <c r="AO1" s="32"/>
+      <c r="AP1" s="32"/>
+      <c r="AQ1" s="32"/>
+      <c r="AR1" s="32"/>
+      <c r="AS1" s="32"/>
+      <c r="AT1" s="32"/>
+      <c r="AU1" s="32"/>
+      <c r="AV1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="AW1" s="7"/>
-      <c r="AX1" s="7"/>
-      <c r="AY1" s="7"/>
-      <c r="AZ1" s="7"/>
-      <c r="BA1" s="7"/>
-      <c r="BB1" s="7"/>
-      <c r="BC1" s="7"/>
-      <c r="BD1" s="6" t="s">
+      <c r="AW1" s="31"/>
+      <c r="AX1" s="31"/>
+      <c r="AY1" s="31"/>
+      <c r="AZ1" s="31"/>
+      <c r="BA1" s="31"/>
+      <c r="BB1" s="31"/>
+      <c r="BC1" s="31"/>
+      <c r="BD1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="BE1" s="6"/>
-      <c r="BF1" s="6"/>
-      <c r="BG1" s="6"/>
-      <c r="BH1" s="6"/>
-      <c r="BI1" s="6"/>
-      <c r="BJ1" s="6"/>
-      <c r="BK1" s="6"/>
-      <c r="BL1" s="5" t="s">
+      <c r="BE1" s="34"/>
+      <c r="BF1" s="34"/>
+      <c r="BG1" s="34"/>
+      <c r="BH1" s="34"/>
+      <c r="BI1" s="34"/>
+      <c r="BJ1" s="34"/>
+      <c r="BK1" s="34"/>
+      <c r="BL1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="BM1" s="5"/>
-      <c r="BN1" s="5"/>
-      <c r="BO1" s="5"/>
-      <c r="BP1" s="5"/>
-      <c r="BQ1" s="5"/>
-      <c r="BR1" s="5"/>
-      <c r="BS1" s="5"/>
-      <c r="BT1" s="4" t="s">
+      <c r="BM1" s="35"/>
+      <c r="BN1" s="35"/>
+      <c r="BO1" s="35"/>
+      <c r="BP1" s="35"/>
+      <c r="BQ1" s="35"/>
+      <c r="BR1" s="35"/>
+      <c r="BS1" s="35"/>
+      <c r="BT1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="BU1" s="4"/>
-      <c r="BV1" s="4"/>
-      <c r="BW1" s="4"/>
-      <c r="BX1" s="4"/>
-      <c r="BY1" s="4"/>
-      <c r="BZ1" s="4"/>
-      <c r="CA1" s="4"/>
-      <c r="CB1" s="3" t="s">
+      <c r="BU1" s="36"/>
+      <c r="BV1" s="36"/>
+      <c r="BW1" s="36"/>
+      <c r="BX1" s="36"/>
+      <c r="BY1" s="36"/>
+      <c r="BZ1" s="36"/>
+      <c r="CA1" s="36"/>
+      <c r="CB1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="CC1" s="3"/>
-      <c r="CD1" s="3"/>
-      <c r="CE1" s="3"/>
-      <c r="CF1" s="3"/>
-      <c r="CG1" s="3"/>
-      <c r="CH1" s="3"/>
-      <c r="CI1" s="3"/>
-      <c r="CJ1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="CK1" s="2"/>
-      <c r="CL1" s="2"/>
-      <c r="CM1" s="2"/>
-      <c r="CN1" s="2"/>
-      <c r="CO1" s="2"/>
-      <c r="CP1" s="2"/>
-      <c r="CQ1" s="2"/>
-      <c r="CR1" s="38" t="s">
+      <c r="CC1" s="37"/>
+      <c r="CD1" s="37"/>
+      <c r="CE1" s="37"/>
+      <c r="CF1" s="37"/>
+      <c r="CG1" s="37"/>
+      <c r="CH1" s="37"/>
+      <c r="CI1" s="37"/>
+      <c r="CJ1" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="CK1" s="38"/>
+      <c r="CL1" s="38"/>
+      <c r="CM1" s="38"/>
+      <c r="CN1" s="38"/>
+      <c r="CO1" s="38"/>
+      <c r="CP1" s="38"/>
+      <c r="CQ1" s="38"/>
+      <c r="CR1" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="CS1" s="38"/>
-      <c r="CT1" s="38"/>
-      <c r="CU1" s="38"/>
-      <c r="CV1" s="38"/>
-      <c r="CW1" s="38"/>
-      <c r="CX1" s="38"/>
-      <c r="CY1" s="39"/>
-      <c r="CZ1" s="7" t="s">
+      <c r="CS1" s="27"/>
+      <c r="CT1" s="27"/>
+      <c r="CU1" s="27"/>
+      <c r="CV1" s="27"/>
+      <c r="CW1" s="27"/>
+      <c r="CX1" s="27"/>
+      <c r="CY1" s="28"/>
+      <c r="CZ1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="DA1" s="7"/>
-      <c r="DB1" s="7"/>
-      <c r="DC1" s="7"/>
-      <c r="DD1" s="7"/>
-      <c r="DE1" s="7"/>
-      <c r="DF1" s="7"/>
-      <c r="DG1" s="7"/>
-      <c r="DH1" s="8" t="s">
+      <c r="DA1" s="31"/>
+      <c r="DB1" s="31"/>
+      <c r="DC1" s="31"/>
+      <c r="DD1" s="31"/>
+      <c r="DE1" s="31"/>
+      <c r="DF1" s="31"/>
+      <c r="DG1" s="31"/>
+      <c r="DH1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="DI1" s="8"/>
-      <c r="DJ1" s="8"/>
-      <c r="DK1" s="8"/>
-      <c r="DL1" s="8"/>
-      <c r="DM1" s="8"/>
-      <c r="DN1" s="8"/>
-      <c r="DO1" s="8"/>
-      <c r="DP1" s="1" t="s">
+      <c r="DI1" s="32"/>
+      <c r="DJ1" s="32"/>
+      <c r="DK1" s="32"/>
+      <c r="DL1" s="32"/>
+      <c r="DM1" s="32"/>
+      <c r="DN1" s="32"/>
+      <c r="DO1" s="32"/>
+      <c r="DP1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="DQ1" s="1"/>
-      <c r="DR1" s="1"/>
-      <c r="DS1" s="1"/>
-      <c r="DT1" s="1"/>
-      <c r="DU1" s="1"/>
-      <c r="DV1" s="1"/>
-      <c r="DW1" s="1"/>
+      <c r="DQ1" s="33"/>
+      <c r="DR1" s="33"/>
+      <c r="DS1" s="33"/>
+      <c r="DT1" s="33"/>
+      <c r="DU1" s="33"/>
+      <c r="DV1" s="33"/>
+      <c r="DW1" s="33"/>
     </row>
     <row r="2" spans="1:127" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="S2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="T2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="U2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="V2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="W2" s="17" t="s">
+      <c r="W2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="X2" s="18" t="s">
+      <c r="X2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="Y2" s="18" t="s">
+      <c r="Y2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" s="18" t="s">
+      <c r="Z2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AA2" s="18" t="s">
+      <c r="AA2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AB2" s="18" t="s">
+      <c r="AB2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="18" t="s">
+      <c r="AC2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AD2" s="18" t="s">
+      <c r="AD2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AE2" s="19" t="s">
+      <c r="AE2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AF2" s="20" t="s">
+      <c r="AF2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AG2" s="20" t="s">
+      <c r="AG2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AH2" s="20" t="s">
+      <c r="AH2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AI2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AJ2" s="20" t="s">
+      <c r="AJ2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AK2" s="20" t="s">
+      <c r="AK2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AL2" s="20" t="s">
+      <c r="AL2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AM2" s="21" t="s">
+      <c r="AM2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="AN2" s="22" t="s">
+      <c r="AN2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AO2" s="22" t="s">
+      <c r="AO2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AP2" s="22" t="s">
+      <c r="AP2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AQ2" s="22" t="s">
+      <c r="AQ2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="AR2" s="22" t="s">
+      <c r="AR2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AS2" s="22" t="s">
+      <c r="AS2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AT2" s="22" t="s">
+      <c r="AT2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AU2" s="23" t="s">
+      <c r="AU2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="AV2" s="24" t="s">
+      <c r="AV2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AW2" s="24" t="s">
+      <c r="AW2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AX2" s="24" t="s">
+      <c r="AX2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AY2" s="24" t="s">
+      <c r="AY2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="AZ2" s="24" t="s">
+      <c r="AZ2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="BA2" s="24" t="s">
+      <c r="BA2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="BB2" s="24" t="s">
+      <c r="BB2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="BC2" s="25" t="s">
+      <c r="BC2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="BD2" s="26" t="s">
+      <c r="BD2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="BE2" s="26" t="s">
+      <c r="BE2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="BF2" s="26" t="s">
+      <c r="BF2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="BG2" s="26" t="s">
+      <c r="BG2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="BH2" s="26" t="s">
+      <c r="BH2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="BI2" s="26" t="s">
+      <c r="BI2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="BJ2" s="26" t="s">
+      <c r="BJ2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="BK2" s="27" t="s">
+      <c r="BK2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="BL2" s="28" t="s">
+      <c r="BL2" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="BM2" s="28" t="s">
+      <c r="BM2" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="BN2" s="28" t="s">
+      <c r="BN2" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="BO2" s="28" t="s">
+      <c r="BO2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="BP2" s="28" t="s">
+      <c r="BP2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="BQ2" s="28" t="s">
+      <c r="BQ2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="BR2" s="28" t="s">
+      <c r="BR2" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="BS2" s="29" t="s">
+      <c r="BS2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="BT2" s="30" t="s">
+      <c r="BT2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="BU2" s="30" t="s">
+      <c r="BU2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="BV2" s="30" t="s">
+      <c r="BV2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="BW2" s="30" t="s">
+      <c r="BW2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="BX2" s="30" t="s">
+      <c r="BX2" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="BY2" s="30" t="s">
+      <c r="BY2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="BZ2" s="30" t="s">
+      <c r="BZ2" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="CA2" s="31" t="s">
+      <c r="CA2" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="CB2" s="32" t="s">
+      <c r="CB2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="CC2" s="32" t="s">
+      <c r="CC2" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="CD2" s="32" t="s">
+      <c r="CD2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="CE2" s="32" t="s">
+      <c r="CE2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="CF2" s="32" t="s">
+      <c r="CF2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="CG2" s="32" t="s">
+      <c r="CG2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="CH2" s="32" t="s">
+      <c r="CH2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="CI2" s="33" t="s">
+      <c r="CI2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="CJ2" s="34" t="s">
+      <c r="CJ2" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="CK2" s="34" t="s">
+      <c r="CK2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="CL2" s="34" t="s">
+      <c r="CL2" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="CM2" s="34" t="s">
+      <c r="CM2" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="CN2" s="34" t="s">
+      <c r="CN2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="CO2" s="34" t="s">
+      <c r="CO2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="CP2" s="34" t="s">
+      <c r="CP2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="CQ2" s="35" t="s">
+      <c r="CQ2" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="CR2" s="40" t="s">
+      <c r="CR2" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="CS2" s="40" t="s">
+      <c r="CS2" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="CT2" s="40" t="s">
+      <c r="CT2" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="CU2" s="40" t="s">
+      <c r="CU2" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="CV2" s="40" t="s">
+      <c r="CV2" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="CW2" s="40" t="s">
+      <c r="CW2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="CX2" s="40" t="s">
+      <c r="CX2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="CY2" s="41" t="s">
+      <c r="CY2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="CZ2" s="24" t="s">
+      <c r="CZ2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="DA2" s="24" t="s">
+      <c r="DA2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="DB2" s="24" t="s">
+      <c r="DB2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="DC2" s="24" t="s">
+      <c r="DC2" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="DD2" s="24" t="s">
+      <c r="DD2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="DE2" s="24" t="s">
+      <c r="DE2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="DF2" s="24" t="s">
+      <c r="DF2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="DG2" s="25" t="s">
+      <c r="DG2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="DH2" s="22" t="s">
+      <c r="DH2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="DI2" s="22" t="s">
+      <c r="DI2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="DJ2" s="22" t="s">
+      <c r="DJ2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="DK2" s="22" t="s">
+      <c r="DK2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="DL2" s="22" t="s">
+      <c r="DL2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="DM2" s="22" t="s">
+      <c r="DM2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="DN2" s="22" t="s">
+      <c r="DN2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="DO2" s="23" t="s">
+      <c r="DO2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="DP2" s="26" t="s">
+      <c r="DP2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="DQ2" s="26" t="s">
+      <c r="DQ2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="DR2" s="26" t="s">
+      <c r="DR2" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="DS2" s="26" t="s">
+      <c r="DS2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="DT2" s="26" t="s">
+      <c r="DT2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="DU2" s="26" t="s">
+      <c r="DU2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="DV2" s="26" t="s">
+      <c r="DV2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="DW2" s="26" t="s">
+      <c r="DW2" s="15" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1490,7 +1503,7 @@
       <c r="V3">
         <v>10</v>
       </c>
-      <c r="W3" s="12">
+      <c r="W3" s="1">
         <v>10</v>
       </c>
       <c r="X3">
@@ -1514,7 +1527,7 @@
       <c r="AD3">
         <v>10</v>
       </c>
-      <c r="AE3" s="12">
+      <c r="AE3" s="1">
         <v>20</v>
       </c>
       <c r="AF3">
@@ -1538,7 +1551,7 @@
       <c r="AL3">
         <v>10</v>
       </c>
-      <c r="AM3" s="12">
+      <c r="AM3" s="1">
         <v>30</v>
       </c>
       <c r="AN3">
@@ -1562,7 +1575,7 @@
       <c r="AT3">
         <v>10</v>
       </c>
-      <c r="AU3" s="12">
+      <c r="AU3" s="1">
         <v>40</v>
       </c>
       <c r="AV3">
@@ -1586,7 +1599,7 @@
       <c r="BB3">
         <v>10</v>
       </c>
-      <c r="BC3" s="12">
+      <c r="BC3" s="1">
         <v>50</v>
       </c>
       <c r="BD3">
@@ -1610,7 +1623,7 @@
       <c r="BJ3">
         <v>10</v>
       </c>
-      <c r="BK3" s="12">
+      <c r="BK3" s="1">
         <v>60</v>
       </c>
       <c r="BL3">
@@ -1634,7 +1647,7 @@
       <c r="BR3">
         <v>10</v>
       </c>
-      <c r="BS3" s="12">
+      <c r="BS3" s="1">
         <v>70</v>
       </c>
       <c r="BT3">
@@ -1658,7 +1671,7 @@
       <c r="BZ3">
         <v>10</v>
       </c>
-      <c r="CA3" s="12">
+      <c r="CA3" s="1">
         <v>80</v>
       </c>
       <c r="CB3">
@@ -1682,7 +1695,7 @@
       <c r="CH3">
         <v>10</v>
       </c>
-      <c r="CI3" s="12">
+      <c r="CI3" s="1">
         <v>90</v>
       </c>
       <c r="CJ3">
@@ -1706,9 +1719,33 @@
       <c r="CP3">
         <v>10</v>
       </c>
-      <c r="CQ3" s="12">
+      <c r="CQ3" s="1">
         <v>100</v>
       </c>
+      <c r="CR3">
+        <v>10</v>
+      </c>
+      <c r="CS3">
+        <v>10</v>
+      </c>
+      <c r="CT3">
+        <v>10</v>
+      </c>
+      <c r="CU3">
+        <v>10</v>
+      </c>
+      <c r="CV3">
+        <v>10</v>
+      </c>
+      <c r="CW3">
+        <v>10</v>
+      </c>
+      <c r="CX3">
+        <v>10</v>
+      </c>
+      <c r="CY3" s="1">
+        <v>110</v>
+      </c>
       <c r="CZ3">
         <v>10</v>
       </c>
@@ -1730,8 +1767,8 @@
       <c r="DF3">
         <v>10</v>
       </c>
-      <c r="DG3" s="12">
-        <v>110</v>
+      <c r="DG3" s="1">
+        <v>120</v>
       </c>
       <c r="DH3">
         <v>10</v>
@@ -1754,8 +1791,8 @@
       <c r="DN3">
         <v>10</v>
       </c>
-      <c r="DO3" s="12">
-        <v>120</v>
+      <c r="DO3" s="42">
+        <v>130</v>
       </c>
       <c r="DP3">
         <v>10</v>
@@ -1779,7 +1816,7 @@
         <v>10</v>
       </c>
       <c r="DW3">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:127" x14ac:dyDescent="0.2">
@@ -1824,10 +1861,15 @@
       </c>
     </row>
     <row r="11" spans="1:127" x14ac:dyDescent="0.2">
-      <c r="E11" s="36"/>
+      <c r="E11" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="P1:W1"/>
+    <mergeCell ref="X1:AE1"/>
+    <mergeCell ref="AF1:AM1"/>
+    <mergeCell ref="AN1:AU1"/>
+    <mergeCell ref="AV1:BC1"/>
     <mergeCell ref="CZ1:DG1"/>
     <mergeCell ref="DH1:DO1"/>
     <mergeCell ref="DP1:DW1"/>
@@ -1836,11 +1878,6 @@
     <mergeCell ref="BT1:CA1"/>
     <mergeCell ref="CB1:CI1"/>
     <mergeCell ref="CJ1:CQ1"/>
-    <mergeCell ref="P1:W1"/>
-    <mergeCell ref="X1:AE1"/>
-    <mergeCell ref="AF1:AM1"/>
-    <mergeCell ref="AN1:AU1"/>
-    <mergeCell ref="AV1:BC1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>